<commit_message>
Code Changes for delettion and update of excel file
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sattu</t>
+          <t>Sattu</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -491,18 +487,12 @@
       <c r="C2" t="n">
         <v>399</v>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G2" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>X00289J163</t>
@@ -512,7 +502,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>sattu</t>
+          <t>Sattu</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -521,18 +511,12 @@
       <c r="C3" t="n">
         <v>599</v>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G3" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
           <t>X00289BZUX</t>
@@ -542,7 +526,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>sattu</t>
+          <t>Sattu</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -551,18 +535,12 @@
       <c r="C4" t="n">
         <v>699</v>
       </c>
-      <c r="D4" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G4" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
           <t>X00289J15T</t>
@@ -572,7 +550,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>sattu</t>
+          <t>Sattu</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -581,18 +559,12 @@
       <c r="C5" t="n">
         <v>799</v>
       </c>
-      <c r="D5" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G5" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
           <t>X00289IWIL</t>
@@ -602,7 +574,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>sattu</t>
+          <t>Sattu</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -611,18 +583,12 @@
       <c r="C6" t="n">
         <v>1099</v>
       </c>
-      <c r="D6" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G6" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>X0029DEJ0L</t>
@@ -651,18 +617,12 @@
       <c r="C8" t="n">
         <v>299</v>
       </c>
-      <c r="D8" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G8" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
           <t>X00289LA0X</t>
@@ -681,18 +641,12 @@
       <c r="C9" t="n">
         <v>399</v>
       </c>
-      <c r="D9" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G9" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
           <t>X00289J14Z</t>
@@ -711,18 +665,12 @@
       <c r="C10" t="n">
         <v>599</v>
       </c>
-      <c r="D10" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G10" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
           <t>X00289HWX7</t>
@@ -741,18 +689,12 @@
       <c r="C11" t="n">
         <v>799</v>
       </c>
-      <c r="D11" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G11" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
           <t>X00289LA0N</t>
@@ -771,18 +713,12 @@
       <c r="C12" t="n">
         <v>899</v>
       </c>
-      <c r="D12" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G12" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
           <t>X00289L9ZT</t>
@@ -802,7 +738,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Govindbhog Rice</t>
+          <t>Govind Bhog Rice</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -811,16 +747,10 @@
       <c r="C14" t="n">
         <v>599</v>
       </c>
-      <c r="D14" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
           <t>X00289IDI5</t>
@@ -830,7 +760,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Govindbhog Rice</t>
+          <t>Govind Bhog Rice</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -839,16 +769,10 @@
       <c r="C15" t="n">
         <v>899</v>
       </c>
-      <c r="D15" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
-      <c r="G15" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
           <t>X00289IDHL</t>
@@ -858,7 +782,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Govindbhog Rice</t>
+          <t>Govind Bhog Rice</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -867,26 +791,16 @@
       <c r="C16" t="n">
         <v>1099</v>
       </c>
-      <c r="D16" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="n">
-        <v>215442</v>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>X00289MEM1</t>
-        </is>
-      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Govindbhog Rice</t>
+          <t>Govind Bhog Rice</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -895,16 +809,10 @@
       <c r="C17" t="n">
         <v>1299</v>
       </c>
-      <c r="D17" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
           <t>X00289MELH</t>
@@ -914,7 +822,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Govindbhog Rice</t>
+          <t>Govind Bhog Rice</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -923,16 +831,10 @@
       <c r="C18" t="n">
         <v>1499</v>
       </c>
-      <c r="D18" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
-      <c r="G18" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
           <t>X002897BI3</t>
@@ -952,7 +854,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Katarni Chuda</t>
+          <t>katarni chuda</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -961,16 +863,10 @@
       <c r="C20" t="n">
         <v>599</v>
       </c>
-      <c r="D20" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
-      <c r="G20" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
           <t>X00289L9ZJ</t>
@@ -980,7 +876,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Katarni Chuda</t>
+          <t>katarni chuda</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -989,16 +885,10 @@
       <c r="C21" t="n">
         <v>899</v>
       </c>
-      <c r="D21" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
           <t>X00289C0YX</t>
@@ -1008,7 +898,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Katarni Chuda</t>
+          <t>katarni chuda</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1017,16 +907,10 @@
       <c r="C22" t="n">
         <v>1499</v>
       </c>
-      <c r="D22" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
-      <c r="G22" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
           <t>X00289J131</t>
@@ -1036,7 +920,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Katarni Chuda</t>
+          <t>katarni chuda</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1045,16 +929,10 @@
       <c r="C23" t="n">
         <v>1699</v>
       </c>
-      <c r="D23" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E23" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
           <t>X00289MR19</t>
@@ -1083,16 +961,10 @@
       <c r="C25" t="n">
         <v>349</v>
       </c>
-      <c r="D25" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
           <t>X00289L64N</t>
@@ -1111,16 +983,10 @@
       <c r="C26" t="n">
         <v>499</v>
       </c>
-      <c r="D26" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
-      <c r="G26" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
           <t>X00289J13L</t>
@@ -1139,16 +1005,10 @@
       <c r="C27" t="n">
         <v>599</v>
       </c>
-      <c r="D27" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
-      <c r="G27" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
           <t>X00289BWA1</t>
@@ -1167,16 +1027,10 @@
       <c r="C28" t="n">
         <v>799</v>
       </c>
-      <c r="D28" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
-      <c r="G28" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
           <t>X0029DDNNF</t>
@@ -1196,114 +1050,78 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Usna Chawal</t>
+          <t>Makhana</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C30" t="n">
-        <v>499</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>45914</v>
-      </c>
+        <v>599</v>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
-      <c r="G30" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>X00289L62Z</t>
+          <t>X00289IWIB</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Usna Chawal</t>
+          <t>Makhana</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="C31" t="n">
-        <v>699</v>
-      </c>
-      <c r="D31" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E31" s="2" t="n">
-        <v>45914</v>
-      </c>
+        <v>999</v>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
-      <c r="G31" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>X00289LA1H</t>
+          <t>X0028FDNJX</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Usna Chawal</t>
+          <t>Makhana</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>0.4</v>
       </c>
       <c r="C32" t="n">
-        <v>899</v>
-      </c>
-      <c r="D32" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E32" s="2" t="n">
-        <v>45914</v>
-      </c>
+        <v>1599</v>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
-      <c r="G32" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>X00289MR23</t>
+          <t>X00289L661</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Usna Chawal</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>4</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1099</v>
-      </c>
-      <c r="D33" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E33" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
-      <c r="G33" t="n">
-        <v>215442</v>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>X00289LA03</t>
-        </is>
-      </c>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1312,284 +1130,236 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C34" t="n">
-        <v>1199</v>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>45914</v>
-      </c>
+        <v>499</v>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
-      <c r="G34" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>X00289HWYB</t>
+          <t>X00289L62Z</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr"/>
-      <c r="B35" t="inlineStr"/>
-      <c r="C35" t="inlineStr"/>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Usna Chawal</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" t="n">
+        <v>699</v>
+      </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>X00289LA1H</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Power punch</t>
+          <t>Usna Chawal</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="C36" t="n">
-        <v>499</v>
-      </c>
-      <c r="D36" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E36" s="2" t="n">
-        <v>45914</v>
-      </c>
+        <v>899</v>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
-      <c r="G36" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>X00289MBPL</t>
+          <t>X00289MR23</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Power punch</t>
+          <t>Usna Chawal</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C37" t="n">
-        <v>899</v>
-      </c>
-      <c r="D37" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E37" s="2" t="n">
-        <v>45914</v>
-      </c>
+        <v>1099</v>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
-      <c r="G37" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>X00289MELR</t>
+          <t>X00289LA03</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Power punch</t>
+          <t>Usna Chawal</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="C38" t="n">
         <v>1199</v>
       </c>
-      <c r="D38" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E38" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
-      <c r="G38" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>X0028FDNBV</t>
+          <t>X00289HWYB</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
         <is>
           <t>Power punch</t>
         </is>
       </c>
-      <c r="B39" t="n">
-        <v>2</v>
-      </c>
-      <c r="C39" t="n">
-        <v>1499</v>
-      </c>
-      <c r="D39" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E39" s="2" t="n">
-        <v>45914</v>
-      </c>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="n">
-        <v>215442</v>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>X0028FDO33</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr"/>
-      <c r="B40" t="inlineStr"/>
-      <c r="C40" t="inlineStr"/>
+      <c r="B40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C40" t="n">
+        <v>499</v>
+      </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>X00289MBPL</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Herbal Gulaal</t>
+          <t>Power punch</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C41" t="n">
-        <v>599</v>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E41" s="2" t="n">
-        <v>45914</v>
-      </c>
+        <v>899</v>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
-      <c r="G41" t="n">
-        <v>215442</v>
-      </c>
+      <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>X00289CAR5</t>
+          <t>X00289MELR</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr"/>
-      <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr"/>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Power punch</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1199</v>
+      </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>X0028FDNBV</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Peri Peri Chana</t>
+          <t>Power punch</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C43" t="n">
-        <v>899</v>
-      </c>
-      <c r="D43" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E43" s="2" t="n">
-        <v>45914</v>
-      </c>
-      <c r="F43" t="n">
-        <v>11117001000101</v>
-      </c>
-      <c r="G43" t="n">
-        <v>215442</v>
-      </c>
+        <v>1499</v>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>X0028N6TEB</t>
+          <t>X0028FDO33</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Peri Peri Chana</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C44" t="n">
-        <v>499</v>
-      </c>
-      <c r="D44" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E44" s="2" t="n">
-        <v>45914</v>
-      </c>
-      <c r="F44" t="n">
-        <v>11117001000101</v>
-      </c>
-      <c r="G44" t="n">
-        <v>215442</v>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>X0028N43VR</t>
-        </is>
-      </c>
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Peri Peri Chana</t>
+          <t>Herbal Gulal</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="C45" t="n">
-        <v>399</v>
-      </c>
-      <c r="D45" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E45" s="2" t="n">
-        <v>45914</v>
-      </c>
-      <c r="F45" t="n">
-        <v>11117001000101</v>
-      </c>
-      <c r="G45" t="n">
-        <v>215442</v>
-      </c>
+        <v>599</v>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>X0028N7S2N</t>
+          <t>X00289CAR5</t>
         </is>
       </c>
     </row>
@@ -1606,7 +1376,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Singhara atta</t>
+          <t>Peri Peri Chana</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1615,24 +1385,22 @@
       <c r="C47" t="n">
         <v>399</v>
       </c>
-      <c r="D47" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E47" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G47" t="n">
-        <v>215442</v>
-      </c>
-      <c r="H47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>X0028N7S2N</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Singhara atta</t>
+          <t>Peri Peri Chana</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1641,24 +1409,22 @@
       <c r="C48" t="n">
         <v>499</v>
       </c>
-      <c r="D48" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E48" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr"/>
       <c r="F48" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G48" t="n">
-        <v>215442</v>
-      </c>
-      <c r="H48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>X0028N43VR</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Singhara atta</t>
+          <t>Peri Peri Chana</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1667,351 +1433,573 @@
       <c r="C49" t="n">
         <v>899</v>
       </c>
-      <c r="D49" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E49" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr"/>
       <c r="F49" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G49" t="n">
-        <v>215442</v>
-      </c>
-      <c r="H49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>X0028N6TEB</t>
+        </is>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Singhara atta</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>2</v>
-      </c>
-      <c r="C50" t="n">
-        <v>1699</v>
-      </c>
-      <c r="D50" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E50" s="2" t="n">
-        <v>45914</v>
-      </c>
-      <c r="F50" t="n">
-        <v>11117001000101</v>
-      </c>
-      <c r="G50" t="n">
-        <v>215442</v>
-      </c>
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr"/>
-      <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr"/>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Cheese &amp; Cream Chana</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C51" t="n">
+        <v>399</v>
+      </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr"/>
+      <c r="F51" t="n">
+        <v>11117001000101</v>
+      </c>
       <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>X002AEZPM5</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Katarni Arwa rice</t>
+          <t>Cheese &amp; Cream Chana</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C52" t="n">
         <v>499</v>
       </c>
-      <c r="D52" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E52" s="2" t="n">
-        <v>45914</v>
-      </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="n">
-        <v>215442</v>
-      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="n">
+        <v>11117001000101</v>
+      </c>
+      <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>X0028ZT5J5</t>
+          <t>X002AEZQUB</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Katarni Arwa rice</t>
+          <t>Cheese &amp; Cream Chana</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53" t="n">
         <v>899</v>
       </c>
-      <c r="D53" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E53" s="2" t="n">
-        <v>45914</v>
-      </c>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="n">
-        <v>215442</v>
-      </c>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="n">
+        <v>11117001000101</v>
+      </c>
+      <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>X0028ZH6ZZ</t>
+          <t>X002AF2WW5</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>Katarni Arwa rice</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>3</v>
-      </c>
-      <c r="C54" t="n">
-        <v>1199</v>
-      </c>
-      <c r="D54" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E54" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
-      <c r="G54" t="n">
-        <v>215442</v>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>X0028ZNEXX</t>
-        </is>
-      </c>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Katarni Arwa rice</t>
+          <t>Nimbu Pudina Chana</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="C55" t="n">
-        <v>1399</v>
-      </c>
-      <c r="D55" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E55" s="2" t="n">
-        <v>45914</v>
-      </c>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="n">
-        <v>215442</v>
-      </c>
+        <v>399</v>
+      </c>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="n">
+        <v>11117001000101</v>
+      </c>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>X0028ZNDG1</t>
+          <t>X002AF43UT</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Katarni Arwa rice</t>
+          <t>Nimbu Pudina Chana</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="C56" t="n">
-        <v>1599</v>
-      </c>
-      <c r="D56" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E56" s="2" t="n">
-        <v>45914</v>
-      </c>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="n">
-        <v>215442</v>
-      </c>
+        <v>499</v>
+      </c>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="n">
+        <v>11117001000101</v>
+      </c>
+      <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>X0028ZN0XH</t>
+          <t>X002AF6W0X</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr"/>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr"/>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Nimbu Pudina Chana</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" t="n">
+        <v>899</v>
+      </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr"/>
+      <c r="F57" t="n">
+        <v>11117001000101</v>
+      </c>
       <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>X002AF02OZ</t>
+        </is>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Jeera Sattu</t>
-        </is>
-      </c>
-      <c r="B58" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C58" t="n">
-        <v>399</v>
-      </c>
-      <c r="D58" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E58" s="2" t="n">
-        <v>45914</v>
-      </c>
-      <c r="F58" t="n">
-        <v>11117001000101</v>
-      </c>
-      <c r="G58" t="n">
-        <v>215442</v>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>X00298E4CJ</t>
-        </is>
-      </c>
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Jeera Sattu</t>
+          <t>Hing Jeera chana</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="C59" t="n">
-        <v>599</v>
-      </c>
-      <c r="D59" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E59" s="2" t="n">
-        <v>45914</v>
-      </c>
+        <v>399</v>
+      </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr"/>
       <c r="F59" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G59" t="n">
-        <v>215442</v>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>X0029889A7</t>
-        </is>
-      </c>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Jeera Sattu</t>
+          <t>Hing Jeera chana</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="C60" t="n">
-        <v>799</v>
-      </c>
-      <c r="D60" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E60" s="2" t="n">
-        <v>45914</v>
-      </c>
+        <v>499</v>
+      </c>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr"/>
       <c r="F60" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G60" t="n">
-        <v>215442</v>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>X00298E6G3</t>
-        </is>
-      </c>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Jeera Sattu</t>
+          <t>Hing Jeera chana</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C61" t="n">
         <v>899</v>
       </c>
-      <c r="D61" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E61" s="2" t="n">
-        <v>45914</v>
-      </c>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr"/>
       <c r="F61" t="n">
         <v>11117001000101</v>
       </c>
-      <c r="G61" t="n">
-        <v>215442</v>
-      </c>
-      <c r="H61" t="inlineStr">
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Singhara atta</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C63" t="n">
+        <v>399</v>
+      </c>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="n">
+        <v>11117001000101</v>
+      </c>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Singhara atta</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C64" t="n">
+        <v>499</v>
+      </c>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="n">
+        <v>11117001000101</v>
+      </c>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Singhara atta</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" t="n">
+        <v>899</v>
+      </c>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="n">
+        <v>11117001000101</v>
+      </c>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Singhara atta</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>2</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1699</v>
+      </c>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="n">
+        <v>11117001000101</v>
+      </c>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Katarni Arwa rice</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1</v>
+      </c>
+      <c r="C68" t="n">
+        <v>499</v>
+      </c>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>X0028ZT5J5</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Katarni Arwa rice</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>2</v>
+      </c>
+      <c r="C69" t="n">
+        <v>899</v>
+      </c>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Katarni Arwa rice</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>3</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1199</v>
+      </c>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>X0028ZNEXX</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Katarni Arwa rice</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>4</v>
+      </c>
+      <c r="C71" t="n">
+        <v>1399</v>
+      </c>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>X0028ZNDG1</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Katarni Arwa rice</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>5</v>
+      </c>
+      <c r="C72" t="n">
+        <v>1599</v>
+      </c>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>X0028ZN0XH</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Jeera Sattu</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C74" t="n">
+        <v>399</v>
+      </c>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>X00298E4CJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Jeera Sattu</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>1</v>
+      </c>
+      <c r="C75" t="n">
+        <v>599</v>
+      </c>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>X0029889A7</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Jeera Sattu</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="C76" t="n">
+        <v>799</v>
+      </c>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="inlineStr"/>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>X00298E6G3</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Jeera Sattu</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>2</v>
+      </c>
+      <c r="C77" t="n">
+        <v>899</v>
+      </c>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr">
         <is>
           <t>X00298E7F3</t>
         </is>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
+    <row r="78">
+      <c r="A78" t="inlineStr">
         <is>
           <t>Jeera Sattu</t>
         </is>
       </c>
-      <c r="B62" t="n">
+      <c r="B78" t="n">
         <v>3</v>
       </c>
-      <c r="C62" t="n">
+      <c r="C78" t="n">
         <v>1199</v>
       </c>
-      <c r="D62" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="E62" s="2" t="n">
-        <v>45914</v>
-      </c>
-      <c r="F62" t="n">
-        <v>11117001000101</v>
-      </c>
-      <c r="G62" t="n">
-        <v>215442</v>
-      </c>
-      <c r="H62" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Commit for Code Changes
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -1637,7 +1637,11 @@
         <v>11117001000101</v>
       </c>
       <c r="G59" t="inlineStr"/>
-      <c r="H59" t="inlineStr"/>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>X002AO7PY1</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1657,7 +1661,11 @@
         <v>11117001000101</v>
       </c>
       <c r="G60" t="inlineStr"/>
-      <c r="H60" t="inlineStr"/>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>X002AOA47V</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1677,7 +1685,11 @@
         <v>11117001000101</v>
       </c>
       <c r="G61" t="inlineStr"/>
-      <c r="H61" t="inlineStr"/>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>X002AO70CD</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr"/>

</xml_diff>